<commit_message>
Update Gini - educ
</commit_message>
<xml_diff>
--- a/GINI_2017.xlsx
+++ b/GINI_2017.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineberleur/Documents/ENS/econometrie/projet_r/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71E7EDB-38FA-F746-A6C2-3D87B347F8FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="22068" windowHeight="9504"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -480,8 +486,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0.##########"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,13 +503,29 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F6F6"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -529,16 +555,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -585,7 +632,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -617,9 +664,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -651,6 +716,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -826,22 +909,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>145</v>
       </c>
@@ -858,7 +941,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -868,8 +951,9 @@
       <c r="C2">
         <v>33.200000000000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -879,8 +963,9 @@
       <c r="C3">
         <v>41.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -890,8 +975,9 @@
       <c r="C4">
         <v>33.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -901,11 +987,14 @@
       <c r="C5">
         <v>29.7</v>
       </c>
+      <c r="D5" s="3">
+        <v>29.7</v>
+      </c>
       <c r="E5" s="2">
         <v>24752</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -915,14 +1004,14 @@
       <c r="C6">
         <v>27.4</v>
       </c>
-      <c r="D6">
-        <v>33.5</v>
+      <c r="D6" s="3">
+        <v>35.6</v>
       </c>
       <c r="E6" s="2">
         <v>22730</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -932,14 +1021,14 @@
       <c r="C7">
         <v>40.4</v>
       </c>
-      <c r="D7">
-        <v>41.6</v>
+      <c r="D7" s="3">
+        <v>24.5</v>
       </c>
       <c r="E7" s="2">
         <v>3588</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -949,8 +1038,9 @@
       <c r="C8">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -960,8 +1050,9 @@
       <c r="C9">
         <v>44.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -971,8 +1062,9 @@
       <c r="C10">
         <v>53.3</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -982,8 +1074,9 @@
       <c r="C11">
         <v>37.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -993,8 +1086,9 @@
       <c r="C12">
         <v>33.299999999999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1004,11 +1098,14 @@
       <c r="C13">
         <v>32.700000000000003</v>
       </c>
+      <c r="D13" s="4">
+        <v>36.799999999999997</v>
+      </c>
       <c r="E13" s="2">
         <v>43663</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1018,8 +1115,9 @@
       <c r="C14">
         <v>44.4</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1029,8 +1127,9 @@
       <c r="C15">
         <v>49.7</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1040,8 +1139,9 @@
       <c r="C16">
         <v>48.3</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1051,11 +1151,14 @@
       <c r="C17">
         <v>31.4</v>
       </c>
+      <c r="D17" s="5">
+        <v>38.1</v>
+      </c>
       <c r="E17" s="2">
         <v>14497</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -1065,14 +1168,14 @@
       <c r="C18">
         <v>24.9</v>
       </c>
-      <c r="D18">
-        <v>32.9</v>
+      <c r="D18" s="5">
+        <v>21.4</v>
       </c>
       <c r="E18" s="2">
         <v>8282</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -1082,8 +1185,9 @@
       <c r="C19">
         <v>41.6</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1093,14 +1197,14 @@
       <c r="C20">
         <v>28.7</v>
       </c>
-      <c r="D20">
-        <v>39.799999999999997</v>
+      <c r="D20" s="4">
+        <v>32.200000000000003</v>
       </c>
       <c r="E20" s="2">
         <v>29383</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
@@ -1110,8 +1214,9 @@
       <c r="C21">
         <v>42.2</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -1121,8 +1226,9 @@
       <c r="C22">
         <v>44.7</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -1132,11 +1238,14 @@
       <c r="C23">
         <v>34.700000000000003</v>
       </c>
+      <c r="D23" s="5">
+        <v>33.200000000000003</v>
+      </c>
       <c r="E23" s="2">
         <v>14207</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
@@ -1146,11 +1255,14 @@
       <c r="C24">
         <v>30.4</v>
       </c>
+      <c r="D24" s="4">
+        <v>34.700000000000003</v>
+      </c>
       <c r="E24" s="2">
         <v>9389</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
@@ -1160,11 +1272,14 @@
       <c r="C25">
         <v>27.4</v>
       </c>
+      <c r="D25" s="4">
+        <v>36.4</v>
+      </c>
       <c r="E25" s="2">
         <v>23987</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
@@ -1174,11 +1289,14 @@
       <c r="C26">
         <v>31.6</v>
       </c>
+      <c r="D26" s="4">
+        <v>31.4</v>
+      </c>
       <c r="E26" s="2">
         <v>21965</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -1188,8 +1306,9 @@
       <c r="C27">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>52</v>
       </c>
@@ -1199,11 +1318,14 @@
       <c r="C28">
         <v>35.1</v>
       </c>
+      <c r="D28" s="5">
+        <v>38.700000000000003</v>
+      </c>
       <c r="E28" s="2">
         <v>20995</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>54</v>
       </c>
@@ -1213,8 +1335,9 @@
       <c r="C29">
         <v>37.9</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>56</v>
       </c>
@@ -1224,11 +1347,14 @@
       <c r="C30">
         <v>34.4</v>
       </c>
+      <c r="D30" s="4">
+        <v>27.2</v>
+      </c>
       <c r="E30" s="2">
         <v>7611</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>58</v>
       </c>
@@ -1238,8 +1364,9 @@
       <c r="C31">
         <v>49.4</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -1249,11 +1376,14 @@
       <c r="C32">
         <v>30.4</v>
       </c>
+      <c r="D32" s="5">
+        <v>20.6</v>
+      </c>
       <c r="E32" s="2">
         <v>6210</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>62</v>
       </c>
@@ -1263,11 +1393,14 @@
       <c r="C33">
         <v>30.6</v>
       </c>
+      <c r="D33" s="5">
+        <v>20.9</v>
+      </c>
       <c r="E33" s="2">
         <v>4993</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>64</v>
       </c>
@@ -1277,8 +1410,9 @@
       <c r="C34">
         <v>38.1</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>66</v>
       </c>
@@ -1288,11 +1422,14 @@
       <c r="C35">
         <v>31.4</v>
       </c>
+      <c r="D35" s="5">
+        <v>40.4</v>
+      </c>
       <c r="E35" s="2">
         <v>22879</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>68</v>
       </c>
@@ -1302,8 +1439,9 @@
       <c r="C36">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>70</v>
       </c>
@@ -1313,11 +1451,14 @@
       <c r="C37">
         <v>26.1</v>
       </c>
+      <c r="D37" s="4">
+        <v>35.299999999999997</v>
+      </c>
       <c r="E37" s="2">
         <v>33839</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
@@ -1327,11 +1468,14 @@
       <c r="C38">
         <v>35.9</v>
       </c>
+      <c r="D38" s="4">
+        <v>16.5</v>
+      </c>
       <c r="E38" s="2">
         <v>16542</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>74</v>
       </c>
@@ -1341,8 +1485,9 @@
       <c r="C39">
         <v>27.5</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>76</v>
       </c>
@@ -1352,8 +1497,9 @@
       <c r="C40">
         <v>27.3</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>78</v>
       </c>
@@ -1363,8 +1509,9 @@
       <c r="C41">
         <v>31.4</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>79</v>
       </c>
@@ -1374,8 +1521,9 @@
       <c r="C42">
         <v>44.9</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>81</v>
       </c>
@@ -1385,11 +1533,14 @@
       <c r="C43">
         <v>37.299999999999997</v>
       </c>
+      <c r="D43" s="5">
+        <v>34.799999999999997</v>
+      </c>
       <c r="E43" s="2">
         <v>6135</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>83</v>
       </c>
@@ -1399,11 +1550,14 @@
       <c r="C44">
         <v>34.5</v>
       </c>
+      <c r="D44" s="4">
+        <v>34.1</v>
+      </c>
       <c r="E44" s="2">
         <v>36321</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>85</v>
       </c>
@@ -1413,11 +1567,14 @@
       <c r="C45">
         <v>35.6</v>
       </c>
+      <c r="D45" s="6">
+        <v>30</v>
+      </c>
       <c r="E45" s="2">
         <v>6607</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>87</v>
       </c>
@@ -1427,8 +1584,9 @@
       <c r="C46">
         <v>25.9</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>89</v>
       </c>
@@ -1438,11 +1596,14 @@
       <c r="C47">
         <v>34.200000000000003</v>
       </c>
+      <c r="D47" s="7">
+        <v>18</v>
+      </c>
       <c r="E47" s="2">
         <v>2439</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>91</v>
       </c>
@@ -1452,11 +1613,14 @@
       <c r="C48">
         <v>29.2</v>
       </c>
+      <c r="D48" s="4">
+        <v>22.1</v>
+      </c>
       <c r="E48" s="2">
         <v>14522</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>93</v>
       </c>
@@ -1466,8 +1630,9 @@
       <c r="C49">
         <v>30.7</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>95</v>
       </c>
@@ -1477,8 +1642,9 @@
       <c r="C50">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>97</v>
       </c>
@@ -1488,11 +1654,14 @@
       <c r="C51">
         <v>28.5</v>
       </c>
+      <c r="D51" s="5">
+        <v>32.1</v>
+      </c>
       <c r="E51" s="2">
         <v>23563</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>99</v>
       </c>
@@ -1502,11 +1671,14 @@
       <c r="C52">
         <v>27</v>
       </c>
+      <c r="D52" s="5">
+        <v>36.799999999999997</v>
+      </c>
       <c r="E52" s="2">
         <v>38494</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>101</v>
       </c>
@@ -1516,8 +1688,9 @@
       <c r="C53">
         <v>49.9</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>103</v>
       </c>
@@ -1527,8 +1700,9 @@
       <c r="C54">
         <v>43.3</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>105</v>
       </c>
@@ -1538,11 +1712,14 @@
       <c r="C55">
         <v>29.7</v>
       </c>
+      <c r="D55" s="5">
+        <v>26.3</v>
+      </c>
       <c r="E55" s="2">
         <v>5960</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>107</v>
       </c>
@@ -1552,11 +1729,14 @@
       <c r="C56">
         <v>33.799999999999997</v>
       </c>
+      <c r="D56" s="4">
+        <v>21.7</v>
+      </c>
       <c r="E56" s="2">
         <v>9071</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>109</v>
       </c>
@@ -1566,8 +1746,9 @@
       <c r="C57">
         <v>48.5</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>111</v>
       </c>
@@ -1577,11 +1758,14 @@
       <c r="C58">
         <v>36</v>
       </c>
+      <c r="D58" s="5">
+        <v>15.3</v>
+      </c>
       <c r="E58" s="2">
         <v>2742</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>113</v>
       </c>
@@ -1591,8 +1775,9 @@
       <c r="C59">
         <v>37.200000000000003</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>115</v>
       </c>
@@ -1602,8 +1787,9 @@
       <c r="C60">
         <v>38</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>117</v>
       </c>
@@ -1613,8 +1799,9 @@
       <c r="C61">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>119</v>
       </c>
@@ -1624,11 +1811,14 @@
       <c r="C62">
         <v>36.200000000000003</v>
       </c>
+      <c r="D62" s="4">
+        <v>19.8</v>
+      </c>
       <c r="E62" s="2">
         <v>2534</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>121</v>
       </c>
@@ -1638,8 +1828,9 @@
       <c r="C63">
         <v>56.3</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>123</v>
       </c>
@@ -1649,11 +1840,14 @@
       <c r="C64">
         <v>24.2</v>
       </c>
+      <c r="D64" s="4">
+        <v>28.7</v>
+      </c>
       <c r="E64" s="2">
         <v>12713</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>125</v>
       </c>
@@ -1663,11 +1857,14 @@
       <c r="C65">
         <v>28.8</v>
       </c>
+      <c r="D65" s="7">
+        <v>36</v>
+      </c>
       <c r="E65" s="2">
         <v>25395</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>127</v>
       </c>
@@ -1677,8 +1874,9 @@
       <c r="C66">
         <v>36.5</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="D66" s="3"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>129</v>
       </c>
@@ -1688,11 +1886,14 @@
       <c r="C67">
         <v>41.4</v>
       </c>
+      <c r="D67" s="5">
+        <v>16.600000000000001</v>
+      </c>
       <c r="E67" s="2">
         <v>3868</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>131</v>
       </c>
@@ -1702,8 +1903,9 @@
       <c r="C68">
         <v>40.5</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="D68" s="3"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>133</v>
       </c>
@@ -1713,8 +1915,9 @@
       <c r="C69">
         <v>26</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="D69" s="3"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>135</v>
       </c>
@@ -1724,8 +1927,9 @@
       <c r="C70">
         <v>39.5</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="D70" s="3"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>137</v>
       </c>
@@ -1735,8 +1939,9 @@
       <c r="C71">
         <v>41.2</v>
       </c>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="D71" s="3"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>139</v>
       </c>
@@ -1746,8 +1951,9 @@
       <c r="C72">
         <v>29</v>
       </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="D72" s="3"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>141</v>
       </c>
@@ -1757,8 +1963,9 @@
       <c r="C73">
         <v>44.3</v>
       </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>147</v>
       </c>
@@ -1768,11 +1975,14 @@
       <c r="C74">
         <v>29.5</v>
       </c>
+      <c r="D74" s="5">
+        <v>24.8</v>
+      </c>
       <c r="E74" s="2">
         <v>21906</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>149</v>
       </c>
@@ -1781,6 +1991,9 @@
       </c>
       <c r="C75">
         <v>25.7</v>
+      </c>
+      <c r="D75" s="3">
+        <v>20.7</v>
       </c>
       <c r="E75" s="2">
         <v>7183</v>
@@ -1793,24 +2006,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>